<commit_message>
teste de animar personagens.
</commit_message>
<xml_diff>
--- a/Editor.xlsx
+++ b/Editor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\MSX_Projetos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2ED685-8D3E-4E84-9E68-CF46B4D1DB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F17BD81-C4C6-4DA1-BE18-B889A205C443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>255,129,129,129,129,129,129,255</t>
   </si>
@@ -127,6 +127,72 @@
   </si>
   <si>
     <t>252,254,254,254,254,254,254,0</t>
+  </si>
+  <si>
+    <t>ESCADA 1</t>
+  </si>
+  <si>
+    <t>ESCADA 2</t>
+  </si>
+  <si>
+    <t>152,191,144,186,159,191,144,176</t>
+  </si>
+  <si>
+    <t>19,247,19,183,243,247,19,23</t>
+  </si>
+  <si>
+    <t>?1</t>
+  </si>
+  <si>
+    <t>?2</t>
+  </si>
+  <si>
+    <t>?3</t>
+  </si>
+  <si>
+    <t>?4</t>
+  </si>
+  <si>
+    <t>255,255,192,199,200,201,199,193</t>
+  </si>
+  <si>
+    <t>254,252,3,227,35,163,163,35</t>
+  </si>
+  <si>
+    <t>194,194,195,194,195,192,127,255</t>
+  </si>
+  <si>
+    <t>67,67,195,67,195,3,255,255</t>
+  </si>
+  <si>
+    <t>8,8,8,24,24,24,24,0</t>
+  </si>
+  <si>
+    <t>124,4,4,28,12,12,124,0</t>
+  </si>
+  <si>
+    <t>124,4,4,124,96,96,124,0</t>
+  </si>
+  <si>
+    <t>68,68,68,124,12,12,12,0</t>
+  </si>
+  <si>
+    <t>120,72,8,24,24,24,24,0</t>
+  </si>
+  <si>
+    <t>124,68,68,124,76,76,124,0</t>
+  </si>
+  <si>
+    <t>124,64,64,124,12,12,124,0</t>
+  </si>
+  <si>
+    <t>124,68,68,124,12,12,12,0</t>
+  </si>
+  <si>
+    <t>124,64,64,124,76,76,124,0</t>
+  </si>
+  <si>
+    <t>124,68,68,76,76,76,124,0</t>
   </si>
 </sst>
 </file>
@@ -266,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -279,7 +345,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -289,17 +354,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color theme="0"/>
@@ -586,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG19"/>
+  <dimension ref="A1:AG35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="AF26" sqref="AF26:AG35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,26 +670,34 @@
       <c r="E1" s="7">
         <v>1</v>
       </c>
-      <c r="F1" s="7">
-        <v>1</v>
-      </c>
+      <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="8"/>
       <c r="I1" s="6"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
+      <c r="J1" s="7">
+        <v>1</v>
+      </c>
+      <c r="K1" s="7">
+        <v>1</v>
+      </c>
+      <c r="L1" s="7">
+        <v>1</v>
+      </c>
+      <c r="M1" s="7">
+        <v>1</v>
+      </c>
+      <c r="N1" s="7">
+        <v>1</v>
+      </c>
       <c r="O1" s="7"/>
       <c r="P1" s="8"/>
       <c r="R1" s="3">
         <f>(H1*$W$1)+(G1*$X$1)+(F1*$Y$1)+(E1*$Z$1) +(D1*$AA$1)+(C1*$AB$1)+(B1*$AC$1)+(A1*$AD$1)</f>
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="S1" s="4">
         <f>(P1*$W$1)+(O1*$X$1)+(N1*$Y$1)+(M1*$Z$1) +(L1*$AA$1)+(K1*$AB$1)+(J1*$AC$1)+(I1*$AD$1)</f>
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="W1" s="1">
         <v>1</v>
@@ -662,87 +725,50 @@
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
-        <v>1</v>
-      </c>
-      <c r="B2" s="10">
-        <v>1</v>
-      </c>
-      <c r="C2" s="10">
-        <v>1</v>
-      </c>
-      <c r="D2" s="10">
-        <v>1</v>
-      </c>
-      <c r="E2" s="10">
-        <v>1</v>
-      </c>
-      <c r="F2" s="10">
-        <v>1</v>
-      </c>
-      <c r="G2" s="10">
-        <v>1</v>
-      </c>
-      <c r="H2" s="11"/>
+      <c r="A2" s="9"/>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="10"/>
       <c r="I2" s="9"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="11"/>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="P2" s="10"/>
       <c r="R2" s="3">
         <f t="shared" ref="R2:R8" si="0">(H2*$W$1)+(G2*$X$1)+(F2*$Y$1)+(E2*$Z$1) +(D2*$AA$1)+(C2*$AB$1)+(B2*$AC$1)+(A2*$AD$1)</f>
-        <v>254</v>
+        <v>72</v>
       </c>
       <c r="S2" s="4">
         <f t="shared" ref="S2:S8" si="1">(P2*$W$1)+(O2*$X$1)+(N2*$Y$1)+(M2*$Z$1) +(L2*$AA$1)+(K2*$AB$1)+(J2*$AC$1)+(I2*$AD$1)</f>
-        <v>0</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
-        <v>1</v>
-      </c>
-      <c r="B3" s="10">
-        <v>1</v>
-      </c>
-      <c r="C3" s="10">
-        <v>1</v>
-      </c>
-      <c r="D3" s="10">
-        <v>1</v>
-      </c>
-      <c r="E3" s="10">
-        <v>1</v>
-      </c>
-      <c r="F3" s="10">
-        <v>1</v>
-      </c>
-      <c r="G3" s="10">
-        <v>1</v>
-      </c>
-      <c r="H3" s="11"/>
+      <c r="A3" s="9"/>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="10"/>
       <c r="I3" s="9"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="11"/>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="P3" s="10"/>
       <c r="R3" s="3">
         <f t="shared" si="0"/>
-        <v>254</v>
+        <v>8</v>
       </c>
       <c r="S3" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="W3" s="3" t="str">
         <f>R1&amp;","&amp;R2&amp;","&amp;R3&amp;","&amp;R4&amp;","&amp;R5&amp;","&amp;R6&amp;","&amp;R7&amp;","&amp;R8</f>
-        <v>124,254,254,254,254,248,240,0</v>
+        <v>120,72,8,24,24,24,24,0</v>
       </c>
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
@@ -757,47 +783,42 @@
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
-        <v>1</v>
-      </c>
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="15">
-        <v>1</v>
-      </c>
-      <c r="D4" s="10">
-        <v>1</v>
-      </c>
-      <c r="E4" s="15">
-        <v>1</v>
-      </c>
-      <c r="F4" s="10">
-        <v>1</v>
-      </c>
-      <c r="G4" s="10">
-        <v>1</v>
-      </c>
-      <c r="H4" s="11"/>
+      <c r="A4" s="9"/>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="10"/>
       <c r="I4" s="9"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="11"/>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="P4" s="10"/>
       <c r="R4" s="3">
         <f t="shared" si="0"/>
-        <v>254</v>
+        <v>24</v>
       </c>
       <c r="S4" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="W4" s="2" t="str">
         <f>R9&amp;","&amp;R10&amp;","&amp;R11&amp;","&amp;R12&amp;","&amp;R13&amp;","&amp;R14&amp;","&amp;R15&amp;","&amp;R16</f>
-        <v>0,0,0,0,0,0,0,0</v>
+        <v>124,68,68,124,76,76,124,0</v>
       </c>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
@@ -812,47 +833,36 @@
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
-        <v>1</v>
-      </c>
-      <c r="B5" s="10">
-        <v>1</v>
-      </c>
-      <c r="C5" s="15">
-        <v>1</v>
-      </c>
-      <c r="D5" s="10">
-        <v>1</v>
-      </c>
-      <c r="E5" s="15">
-        <v>1</v>
-      </c>
-      <c r="F5" s="10">
-        <v>1</v>
-      </c>
-      <c r="G5" s="15">
-        <v>1</v>
-      </c>
-      <c r="H5" s="11"/>
+      <c r="A5" s="9"/>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="10"/>
       <c r="I5" s="9"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="11"/>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="P5" s="10"/>
       <c r="R5" s="3">
         <f t="shared" si="0"/>
-        <v>254</v>
+        <v>24</v>
       </c>
       <c r="S5" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="W5" s="4" t="str">
         <f>S1&amp;","&amp;S2&amp;","&amp;S3&amp;","&amp;S4&amp;","&amp;S5&amp;","&amp;S6&amp;","&amp;S7&amp;","&amp;S8</f>
-        <v>0,0,0,0,0,0,0,0</v>
+        <v>124,64,64,124,76,76,124,0</v>
       </c>
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
@@ -867,43 +877,36 @@
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
-        <v>1</v>
-      </c>
-      <c r="B6" s="15">
-        <v>1</v>
-      </c>
-      <c r="C6" s="15">
-        <v>1</v>
-      </c>
-      <c r="D6" s="10">
-        <v>1</v>
-      </c>
-      <c r="E6" s="15">
-        <v>1</v>
-      </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="11"/>
+      <c r="A6" s="9"/>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="10"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="11"/>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="P6" s="10"/>
       <c r="R6" s="3">
         <f t="shared" si="0"/>
-        <v>248</v>
+        <v>24</v>
       </c>
       <c r="S6" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="W6" s="5" t="str">
         <f>S9&amp;","&amp;S10&amp;","&amp;S11&amp;","&amp;S12&amp;","&amp;S13&amp;","&amp;S14&amp;","&amp;S15&amp;","&amp;S16</f>
-        <v>0,0,0,0,0,0,0,0</v>
+        <v>124,68,68,76,76,76,124,0</v>
       </c>
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
@@ -918,37 +921,38 @@
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <v>1</v>
-      </c>
-      <c r="B7" s="15">
-        <v>1</v>
-      </c>
-      <c r="C7" s="15">
-        <v>1</v>
-      </c>
-      <c r="D7" s="15">
-        <v>1</v>
-      </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="11"/>
+      <c r="A7" s="9"/>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="10"/>
       <c r="I7" s="9"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="11"/>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7" s="14">
+        <v>1</v>
+      </c>
+      <c r="P7" s="10"/>
       <c r="R7" s="3">
         <f t="shared" si="0"/>
-        <v>240</v>
+        <v>24</v>
       </c>
       <c r="S7" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="AF7" t="s">
         <v>11</v>
@@ -958,22 +962,22 @@
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="14"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="13"/>
       <c r="R8" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -991,28 +995,48 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
+        <v>1</v>
+      </c>
       <c r="G9" s="7"/>
       <c r="H9" s="8"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
+      <c r="J9" s="7">
+        <v>1</v>
+      </c>
+      <c r="K9" s="7">
+        <v>1</v>
+      </c>
+      <c r="L9" s="7">
+        <v>1</v>
+      </c>
+      <c r="M9" s="7">
+        <v>1</v>
+      </c>
+      <c r="N9" s="7">
+        <v>1</v>
+      </c>
       <c r="O9" s="7"/>
       <c r="P9" s="8"/>
       <c r="R9" s="2">
         <f>(H9*$W$1)+(G9*$X$1)+(F9*$Y$1)+(E9*$Z$1) +(D9*$AA$1)+(C9*$AB$1)+(B9*$AC$1)+(A9*$AD$1)</f>
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="S9" s="5">
         <f>(P9*$W$1)+(O9*$X$1)+(N9*$Y$1)+(M9*$Z$1) +(L9*$AA$1)+(K9*$AB$1)+(J9*$AC$1)+(I9*$AD$1)</f>
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="AF9" t="s">
         <v>13</v>
@@ -1023,28 +1047,28 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11"/>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="10"/>
       <c r="I10" s="9"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="11"/>
+      <c r="J10" s="14">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="P10" s="10"/>
       <c r="R10" s="2">
         <f t="shared" ref="R10:R16" si="2">(H10*$W$1)+(G10*$X$1)+(F10*$Y$1)+(E10*$Z$1) +(D10*$AA$1)+(C10*$AB$1)+(B10*$AC$1)+(A10*$AD$1)</f>
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="S10" s="5">
         <f t="shared" ref="S10:S16" si="3">(P10*$W$1)+(O10*$X$1)+(N10*$Y$1)+(M10*$Z$1) +(L10*$AA$1)+(K10*$AB$1)+(J10*$AC$1)+(I10*$AD$1)</f>
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="AF10" t="s">
         <v>14</v>
@@ -1055,28 +1079,28 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11"/>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="H11" s="10"/>
       <c r="I11" s="9"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="11"/>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="P11" s="10"/>
       <c r="R11" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="S11" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="AF11" t="s">
         <v>17</v>
@@ -1087,28 +1111,40 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="11"/>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="H12" s="10"/>
       <c r="I12" s="9"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="11"/>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="P12" s="10"/>
       <c r="R12" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="S12" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="AF12" t="s">
         <v>18</v>
@@ -1119,28 +1155,34 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="11"/>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="H13" s="10"/>
       <c r="I13" s="9"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="11"/>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="P13" s="10"/>
       <c r="R13" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="S13" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="AF13" t="s">
         <v>19</v>
@@ -1151,28 +1193,34 @@
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="11"/>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="H14" s="10"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="11"/>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="P14" s="10"/>
       <c r="R14" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="S14" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="AF14" t="s">
         <v>20</v>
@@ -1183,28 +1231,46 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="11"/>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="H15" s="10"/>
       <c r="I15" s="9"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="11"/>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="P15" s="10"/>
       <c r="R15" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="S15" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="AF15" t="s">
         <v>21</v>
@@ -1214,22 +1280,22 @@
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="14"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="13"/>
       <c r="R16" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1269,14 +1335,137 @@
         <v>33</v>
       </c>
     </row>
+    <row r="20" spans="32:33" x14ac:dyDescent="0.25">
+      <c r="AF20" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="32:33" x14ac:dyDescent="0.25">
+      <c r="AF21" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="32:33" x14ac:dyDescent="0.25">
+      <c r="AF22" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="32:33" x14ac:dyDescent="0.25">
+      <c r="AF23" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="32:33" x14ac:dyDescent="0.25">
+      <c r="AF24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="32:33" x14ac:dyDescent="0.25">
+      <c r="AF25" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="32:33" x14ac:dyDescent="0.25">
+      <c r="AF26">
+        <v>1</v>
+      </c>
+      <c r="AG26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="32:33" x14ac:dyDescent="0.25">
+      <c r="AF27">
+        <v>2</v>
+      </c>
+      <c r="AG27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="32:33" x14ac:dyDescent="0.25">
+      <c r="AF28">
+        <v>3</v>
+      </c>
+      <c r="AG28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="32:33" x14ac:dyDescent="0.25">
+      <c r="AF29">
+        <v>4</v>
+      </c>
+      <c r="AG29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="32:33" x14ac:dyDescent="0.25">
+      <c r="AF30">
+        <v>5</v>
+      </c>
+      <c r="AG30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="32:33" x14ac:dyDescent="0.25">
+      <c r="AF31">
+        <v>6</v>
+      </c>
+      <c r="AG31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="32:33" x14ac:dyDescent="0.25">
+      <c r="AF32">
+        <v>7</v>
+      </c>
+      <c r="AG32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="32:33" x14ac:dyDescent="0.25">
+      <c r="AF33">
+        <v>8</v>
+      </c>
+      <c r="AG33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="32:33" x14ac:dyDescent="0.25">
+      <c r="AF34">
+        <v>9</v>
+      </c>
+      <c r="AG34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="32:33" x14ac:dyDescent="0.25">
+      <c r="AF35">
+        <v>0</v>
+      </c>
+      <c r="AG35" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A15:I15 P15 A16:P16 A1:P14">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K15:N15">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="A1:P16">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
alteracao de nivel e inclusao de inimigos.
</commit_message>
<xml_diff>
--- a/Editor.xlsx
+++ b/Editor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\MSX_Projetos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D8BA0F-1C1F-4A56-BABF-27A19E0F3F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6394E859-5E46-4162-AE77-79283BB11F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2265" yWindow="1890" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -332,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -350,11 +350,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -641,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG35"/>
+  <dimension ref="A1:AG51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,39 +680,33 @@
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
-      <c r="C1" s="7">
-        <v>1</v>
-      </c>
-      <c r="D1" s="7">
-        <v>1</v>
-      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="E1" s="7">
         <v>1</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="F1" s="7">
+        <v>1</v>
+      </c>
+      <c r="G1" s="7">
+        <v>1</v>
+      </c>
       <c r="H1" s="8"/>
       <c r="I1" s="6"/>
       <c r="J1" s="7"/>
-      <c r="K1" s="14">
-        <v>1</v>
-      </c>
-      <c r="L1" s="7">
-        <v>1</v>
-      </c>
-      <c r="M1" s="7">
-        <v>1</v>
-      </c>
+      <c r="K1" s="14"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
       <c r="P1" s="8"/>
       <c r="R1" s="3">
         <f>(H1*$W$1)+(G1*$X$1)+(F1*$Y$1)+(E1*$Z$1) +(D1*$AA$1)+(C1*$AB$1)+(B1*$AC$1)+(A1*$AD$1)</f>
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="S1" s="4">
         <f>(P1*$W$1)+(O1*$X$1)+(N1*$Y$1)+(M1*$Z$1) +(L1*$AA$1)+(K1*$AB$1)+(J1*$AC$1)+(I1*$AD$1)</f>
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="W1" s="1">
         <v>1</v>
@@ -720,46 +735,66 @@
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="C2">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="9"/>
-      <c r="M2">
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="15">
         <v>1</v>
       </c>
       <c r="P2" s="10"/>
       <c r="R2" s="3">
         <f t="shared" ref="R2:R8" si="0">(H2*$W$1)+(G2*$X$1)+(F2*$Y$1)+(E2*$Z$1) +(D2*$AA$1)+(C2*$AB$1)+(B2*$AC$1)+(A2*$AD$1)</f>
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="S2" s="4">
         <f t="shared" ref="S2:S8" si="1">(P2*$W$1)+(O2*$X$1)+(N2*$Y$1)+(M2*$Z$1) +(L2*$AA$1)+(K2*$AB$1)+(J2*$AC$1)+(I2*$AD$1)</f>
-        <v>8</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="9"/>
-      <c r="M3">
-        <v>1</v>
-      </c>
+      <c r="E3" s="15">
+        <v>1</v>
+      </c>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15">
+        <v>1</v>
+      </c>
+      <c r="H3" s="10">
+        <v>1</v>
+      </c>
+      <c r="I3" s="9">
+        <v>1</v>
+      </c>
+      <c r="J3" s="15">
+        <v>1</v>
+      </c>
+      <c r="K3" s="15">
+        <v>1</v>
+      </c>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
       <c r="P3" s="10"/>
       <c r="R3" s="3">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="S3" s="4">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>224</v>
       </c>
       <c r="W3" s="3" t="str">
         <f>R1&amp;","&amp;R2&amp;","&amp;R3&amp;","&amp;R4&amp;","&amp;R5&amp;","&amp;R6&amp;","&amp;R7&amp;","&amp;R8</f>
-        <v>56,32,32,32,32,32,32,56</v>
+        <v>14,6,11,31,31,15,1,7</v>
       </c>
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
@@ -775,26 +810,44 @@
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="9"/>
-      <c r="M4">
-        <v>1</v>
-      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="15">
+        <v>1</v>
+      </c>
+      <c r="H4" s="10">
+        <v>1</v>
+      </c>
+      <c r="I4" s="9">
+        <v>1</v>
+      </c>
+      <c r="J4" s="15">
+        <v>1</v>
+      </c>
+      <c r="K4" s="15">
+        <v>1</v>
+      </c>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
       <c r="P4" s="10"/>
       <c r="R4" s="3">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S4" s="4">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>224</v>
       </c>
       <c r="W4" s="2" t="str">
         <f>R9&amp;","&amp;R10&amp;","&amp;R11&amp;","&amp;R12&amp;","&amp;R13&amp;","&amp;R14&amp;","&amp;R15&amp;","&amp;R16</f>
-        <v>0,0,0,0,0,0,0,0</v>
+        <v>15,15,0,0,48,60,30,14</v>
       </c>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
@@ -810,26 +863,43 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="9"/>
-      <c r="M5">
-        <v>1</v>
-      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="15">
+        <v>1</v>
+      </c>
+      <c r="G5" s="15">
+        <v>1</v>
+      </c>
+      <c r="H5" s="10">
+        <v>1</v>
+      </c>
+      <c r="I5" s="9">
+        <v>1</v>
+      </c>
+      <c r="J5" s="15">
+        <v>1</v>
+      </c>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
       <c r="P5" s="10"/>
       <c r="R5" s="3">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S5" s="4">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>192</v>
       </c>
       <c r="W5" s="4" t="str">
         <f>S1&amp;","&amp;S2&amp;","&amp;S3&amp;","&amp;S4&amp;","&amp;S5&amp;","&amp;S6&amp;","&amp;S7&amp;","&amp;S8</f>
-        <v>56,8,8,8,8,8,8,56</v>
+        <v>0,96,224,224,192,128,192,248</v>
       </c>
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
@@ -845,26 +915,33 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="9"/>
-      <c r="M6">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="15">
+        <v>1</v>
+      </c>
+      <c r="G6" s="15">
+        <v>1</v>
+      </c>
+      <c r="H6" s="10">
+        <v>1</v>
+      </c>
+      <c r="I6" s="9">
         <v>1</v>
       </c>
       <c r="P6" s="10"/>
       <c r="R6" s="3">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="S6" s="4">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="W6" s="5" t="str">
         <f>S9&amp;","&amp;S10&amp;","&amp;S11&amp;","&amp;S12&amp;","&amp;S13&amp;","&amp;S14&amp;","&amp;S15&amp;","&amp;S16</f>
-        <v>0,0,0,0,0,0,0,0</v>
+        <v>184,190,28,28,0,60,60,120</v>
       </c>
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
@@ -880,22 +957,23 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="9"/>
-      <c r="M7">
+      <c r="H7" s="10">
+        <v>1</v>
+      </c>
+      <c r="I7" s="9">
+        <v>1</v>
+      </c>
+      <c r="J7">
         <v>1</v>
       </c>
       <c r="P7" s="10"/>
       <c r="R7" s="3">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="S7" s="4">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>192</v>
       </c>
       <c r="AF7" t="s">
         <v>11</v>
@@ -907,20 +985,24 @@
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="12"/>
-      <c r="C8" s="12">
-        <v>1</v>
-      </c>
-      <c r="D8" s="12">
-        <v>1</v>
-      </c>
-      <c r="E8" s="12">
-        <v>1</v>
-      </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12">
+        <v>1</v>
+      </c>
+      <c r="G8" s="12">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <v>1</v>
+      </c>
+      <c r="I8" s="11">
+        <v>1</v>
+      </c>
+      <c r="J8" s="12">
+        <v>1</v>
+      </c>
       <c r="K8" s="12">
         <v>1</v>
       </c>
@@ -935,11 +1017,11 @@
       <c r="P8" s="13"/>
       <c r="R8" s="3">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="S8" s="4">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>248</v>
       </c>
       <c r="AF8" t="s">
         <v>12</v>
@@ -953,25 +1035,41 @@
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="6"/>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
+        <v>1</v>
+      </c>
+      <c r="G9" s="7">
+        <v>1</v>
+      </c>
+      <c r="H9" s="8">
+        <v>1</v>
+      </c>
+      <c r="I9" s="6">
+        <v>1</v>
+      </c>
       <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
+      <c r="K9" s="7">
+        <v>1</v>
+      </c>
+      <c r="L9" s="7">
+        <v>1</v>
+      </c>
+      <c r="M9" s="7">
+        <v>1</v>
+      </c>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="8"/>
       <c r="R9" s="2">
         <f>(H9*$W$1)+(G9*$X$1)+(F9*$Y$1)+(E9*$Z$1) +(D9*$AA$1)+(C9*$AB$1)+(B9*$AC$1)+(A9*$AD$1)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="S9" s="5">
         <f>(P9*$W$1)+(O9*$X$1)+(N9*$Y$1)+(M9*$Z$1) +(L9*$AA$1)+(K9*$AB$1)+(J9*$AC$1)+(I9*$AD$1)</f>
-        <v>0</v>
+        <v>184</v>
       </c>
       <c r="AF9" t="s">
         <v>13</v>
@@ -982,16 +1080,44 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="9"/>
+      <c r="E10" s="15">
+        <v>1</v>
+      </c>
+      <c r="F10" s="15">
+        <v>1</v>
+      </c>
+      <c r="G10" s="15">
+        <v>1</v>
+      </c>
+      <c r="H10" s="10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="9">
+        <v>1</v>
+      </c>
+      <c r="K10" s="15">
+        <v>1</v>
+      </c>
+      <c r="L10" s="15">
+        <v>1</v>
+      </c>
+      <c r="M10" s="15">
+        <v>1</v>
+      </c>
+      <c r="N10" s="15">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
       <c r="P10" s="10"/>
       <c r="R10" s="2">
         <f t="shared" ref="R10:R16" si="2">(H10*$W$1)+(G10*$X$1)+(F10*$Y$1)+(E10*$Z$1) +(D10*$AA$1)+(C10*$AB$1)+(B10*$AC$1)+(A10*$AD$1)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="S10" s="5">
         <f t="shared" ref="S10:S16" si="3">(P10*$W$1)+(O10*$X$1)+(N10*$Y$1)+(M10*$Z$1) +(L10*$AA$1)+(K10*$AB$1)+(J10*$AC$1)+(I10*$AD$1)</f>
-        <v>0</v>
+        <v>190</v>
       </c>
       <c r="AF10" t="s">
         <v>14</v>
@@ -1004,6 +1130,16 @@
       <c r="A11" s="9"/>
       <c r="H11" s="10"/>
       <c r="I11" s="9"/>
+      <c r="J11" s="15"/>
+      <c r="L11" s="15">
+        <v>1</v>
+      </c>
+      <c r="M11" s="15">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
       <c r="P11" s="10"/>
       <c r="R11" s="2">
         <f t="shared" si="2"/>
@@ -1011,7 +1147,7 @@
       </c>
       <c r="S11" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AF11" t="s">
         <v>17</v>
@@ -1022,8 +1158,21 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
       <c r="H12" s="10"/>
       <c r="I12" s="9"/>
+      <c r="J12" s="15"/>
+      <c r="L12" s="15">
+        <v>1</v>
+      </c>
+      <c r="M12" s="15">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
       <c r="P12" s="10"/>
       <c r="R12" s="2">
         <f t="shared" si="2"/>
@@ -1031,7 +1180,7 @@
       </c>
       <c r="S12" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AF12" t="s">
         <v>18</v>
@@ -1042,12 +1191,18 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
       <c r="H13" s="10"/>
       <c r="I13" s="9"/>
       <c r="P13" s="10"/>
       <c r="R13" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="S13" s="5">
         <f t="shared" si="3"/>
@@ -1062,16 +1217,41 @@
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="15">
+        <v>1</v>
+      </c>
       <c r="H14" s="10"/>
       <c r="I14" s="9"/>
+      <c r="J14" s="15"/>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14" s="15">
+        <v>1</v>
+      </c>
       <c r="P14" s="10"/>
       <c r="R14" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="S14" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="AF14" t="s">
         <v>20</v>
@@ -1082,16 +1262,40 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
       <c r="H15" s="10"/>
       <c r="I15" s="9"/>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15" s="15">
+        <v>1</v>
+      </c>
       <c r="P15" s="10"/>
       <c r="R15" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="S15" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="AF15" t="s">
         <v>21</v>
@@ -1105,25 +1309,39 @@
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+      <c r="E16" s="12">
+        <v>1</v>
+      </c>
+      <c r="F16" s="12">
+        <v>1</v>
+      </c>
+      <c r="G16" s="12">
+        <v>1</v>
+      </c>
       <c r="H16" s="13"/>
       <c r="I16" s="11"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
+      <c r="J16" s="12">
+        <v>1</v>
+      </c>
+      <c r="K16" s="12">
+        <v>1</v>
+      </c>
+      <c r="L16" s="12">
+        <v>1</v>
+      </c>
+      <c r="M16" s="12">
+        <v>1</v>
+      </c>
       <c r="N16" s="12"/>
       <c r="O16" s="12"/>
       <c r="P16" s="13"/>
       <c r="R16" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="S16" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="AF16" t="s">
         <v>22</v>
@@ -1132,7 +1350,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="32:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="AF17" t="s">
         <v>23</v>
       </c>
@@ -1140,7 +1358,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="32:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="AF18" t="s">
         <v>24</v>
       </c>
@@ -1148,7 +1366,43 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="32:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7">
+        <v>1</v>
+      </c>
+      <c r="D19" s="7">
+        <v>1</v>
+      </c>
+      <c r="E19" s="7">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7">
+        <v>1</v>
+      </c>
+      <c r="G19" s="7">
+        <v>1</v>
+      </c>
+      <c r="H19" s="8">
+        <v>1</v>
+      </c>
+      <c r="I19" s="6">
+        <v>1</v>
+      </c>
+      <c r="J19" s="7"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7">
+        <v>1</v>
+      </c>
+      <c r="N19" s="7">
+        <v>1</v>
+      </c>
+      <c r="O19" s="7">
+        <v>1</v>
+      </c>
+      <c r="P19" s="8"/>
       <c r="AF19" t="s">
         <v>25</v>
       </c>
@@ -1156,7 +1410,33 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="32:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="H20" s="10">
+        <v>1</v>
+      </c>
+      <c r="I20" s="9">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20" s="15">
+        <v>1</v>
+      </c>
+      <c r="N20" s="15">
+        <v>1</v>
+      </c>
+      <c r="P20" s="10"/>
       <c r="AF20" t="s">
         <v>34</v>
       </c>
@@ -1164,7 +1444,31 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="32:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="15">
+        <v>1</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15">
+        <v>1</v>
+      </c>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15">
+        <v>1</v>
+      </c>
+      <c r="N21" s="15"/>
+      <c r="P21" s="10"/>
       <c r="AF21" t="s">
         <v>35</v>
       </c>
@@ -1172,7 +1476,20 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="32:33" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="15">
+        <v>1</v>
+      </c>
+      <c r="H22" s="10"/>
+      <c r="I22" s="9"/>
+      <c r="N22" s="15">
+        <v>1</v>
+      </c>
+      <c r="P22" s="10"/>
       <c r="AF22" t="s">
         <v>38</v>
       </c>
@@ -1180,7 +1497,25 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="32:33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="E23" s="15">
+        <v>1</v>
+      </c>
+      <c r="F23" s="15">
+        <v>1</v>
+      </c>
+      <c r="G23" s="15"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15">
+        <v>1</v>
+      </c>
+      <c r="P23" s="10"/>
       <c r="AF23" t="s">
         <v>39</v>
       </c>
@@ -1188,7 +1523,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="32:33" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" s="10"/>
+      <c r="I24" s="9"/>
+      <c r="M24" s="15">
+        <v>1</v>
+      </c>
+      <c r="P24" s="10"/>
       <c r="AF24" t="s">
         <v>40</v>
       </c>
@@ -1196,7 +1544,29 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="32:33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="H25" s="10"/>
+      <c r="I25" s="9"/>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="P25" s="10"/>
       <c r="AF25" t="s">
         <v>41</v>
       </c>
@@ -1204,7 +1574,27 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="32:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12">
+        <v>1</v>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12">
+        <v>1</v>
+      </c>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="13"/>
       <c r="AF26">
         <v>1</v>
       </c>
@@ -1212,7 +1602,29 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="32:33" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7">
+        <v>1</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7">
+        <v>1</v>
+      </c>
+      <c r="H27" s="8"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7">
+        <v>1</v>
+      </c>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="8"/>
       <c r="AF27">
         <v>2</v>
       </c>
@@ -1220,7 +1632,20 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="32:33" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28" s="10"/>
+      <c r="I28" s="9"/>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="P28" s="10"/>
       <c r="AF28">
         <v>3</v>
       </c>
@@ -1228,7 +1653,36 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="32:33" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29" s="10">
+        <v>1</v>
+      </c>
+      <c r="I29" s="9">
+        <v>1</v>
+      </c>
+      <c r="J29" s="15">
+        <v>1</v>
+      </c>
+      <c r="K29" s="15">
+        <v>1</v>
+      </c>
+      <c r="L29" s="15">
+        <v>1</v>
+      </c>
+      <c r="M29" s="15">
+        <v>1</v>
+      </c>
+      <c r="P29" s="10"/>
       <c r="AF29">
         <v>4</v>
       </c>
@@ -1236,7 +1690,42 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="32:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30" s="10">
+        <v>1</v>
+      </c>
+      <c r="I30" s="9">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30" s="15">
+        <v>1</v>
+      </c>
+      <c r="M30" s="15">
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+      <c r="O30">
+        <v>1</v>
+      </c>
+      <c r="P30" s="10"/>
       <c r="AF30">
         <v>5</v>
       </c>
@@ -1244,7 +1733,44 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="32:33" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" s="15">
+        <v>1</v>
+      </c>
+      <c r="G31" s="15">
+        <v>1</v>
+      </c>
+      <c r="H31" s="10">
+        <v>1</v>
+      </c>
+      <c r="I31" s="9">
+        <v>1</v>
+      </c>
+      <c r="J31" s="15">
+        <v>1</v>
+      </c>
+      <c r="K31" s="15">
+        <v>1</v>
+      </c>
+      <c r="L31" s="15">
+        <v>1</v>
+      </c>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15">
+        <v>1</v>
+      </c>
+      <c r="P31" s="10"/>
       <c r="AF31">
         <v>6</v>
       </c>
@@ -1252,7 +1778,27 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="32:33" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A32" s="9"/>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="G32" s="15">
+        <v>1</v>
+      </c>
+      <c r="H32" s="10">
+        <v>1</v>
+      </c>
+      <c r="I32" s="9">
+        <v>1</v>
+      </c>
+      <c r="J32" s="15">
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32" s="10"/>
       <c r="AF32">
         <v>7</v>
       </c>
@@ -1260,7 +1806,22 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="32:33" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33" s="10"/>
+      <c r="I33" s="9">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
+      <c r="P33" s="10"/>
       <c r="AF33">
         <v>8</v>
       </c>
@@ -1268,7 +1829,31 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="32:33" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12">
+        <v>1</v>
+      </c>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="13">
+        <v>1</v>
+      </c>
+      <c r="I34" s="11">
+        <v>1</v>
+      </c>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12">
+        <v>1</v>
+      </c>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+      <c r="P34" s="13"/>
       <c r="AF34">
         <v>9</v>
       </c>
@@ -1276,7 +1861,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="32:33" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="AF35">
         <v>0</v>
       </c>
@@ -1284,8 +1869,415 @@
         <v>55</v>
       </c>
     </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="7">
+        <v>1</v>
+      </c>
+      <c r="C36" s="7">
+        <v>1</v>
+      </c>
+      <c r="D36" s="7">
+        <v>1</v>
+      </c>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="8">
+        <v>1</v>
+      </c>
+      <c r="I36" s="6">
+        <v>1</v>
+      </c>
+      <c r="J36" s="7">
+        <v>1</v>
+      </c>
+      <c r="K36" s="14">
+        <v>1</v>
+      </c>
+      <c r="L36" s="7">
+        <v>1</v>
+      </c>
+      <c r="M36" s="7">
+        <v>1</v>
+      </c>
+      <c r="N36" s="7">
+        <v>1</v>
+      </c>
+      <c r="O36" s="7"/>
+      <c r="P36" s="8"/>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A37" s="9"/>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="H37" s="10">
+        <v>1</v>
+      </c>
+      <c r="I37" s="9">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
+      <c r="P37" s="10"/>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A38" s="9"/>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15">
+        <v>1</v>
+      </c>
+      <c r="G38" s="15"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15">
+        <v>1</v>
+      </c>
+      <c r="M38" s="15">
+        <v>1</v>
+      </c>
+      <c r="N38" s="15">
+        <v>1</v>
+      </c>
+      <c r="P38" s="10"/>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A39" s="9"/>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="H39" s="10"/>
+      <c r="I39" s="9"/>
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39" s="15">
+        <v>1</v>
+      </c>
+      <c r="N39" s="15"/>
+      <c r="P39" s="10"/>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A40" s="9"/>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15">
+        <v>1</v>
+      </c>
+      <c r="L40" s="15">
+        <v>1</v>
+      </c>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="P40" s="10"/>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A41" s="9"/>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="H41" s="10"/>
+      <c r="I41" s="9"/>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="P41" s="10"/>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A42" s="9"/>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42" s="10"/>
+      <c r="I42" s="9"/>
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="P42" s="10"/>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12">
+        <v>1</v>
+      </c>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="12"/>
+      <c r="K43" s="12"/>
+      <c r="L43" s="12"/>
+      <c r="M43" s="12"/>
+      <c r="N43" s="12">
+        <v>1</v>
+      </c>
+      <c r="O43" s="12"/>
+      <c r="P43" s="13"/>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7">
+        <v>1</v>
+      </c>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="7">
+        <v>1</v>
+      </c>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7">
+        <v>1</v>
+      </c>
+      <c r="O44" s="7"/>
+      <c r="P44" s="8"/>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A45" s="9"/>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="H45" s="10"/>
+      <c r="I45" s="9"/>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="O45">
+        <v>1</v>
+      </c>
+      <c r="P45" s="10"/>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A46" s="9"/>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46" s="10">
+        <v>1</v>
+      </c>
+      <c r="I46" s="9">
+        <v>1</v>
+      </c>
+      <c r="J46" s="15">
+        <v>1</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="O46">
+        <v>1</v>
+      </c>
+      <c r="P46" s="10"/>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A47" s="9"/>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47" s="15">
+        <v>1</v>
+      </c>
+      <c r="F47" s="15">
+        <v>1</v>
+      </c>
+      <c r="G47" s="15">
+        <v>1</v>
+      </c>
+      <c r="H47" s="10">
+        <v>1</v>
+      </c>
+      <c r="I47" s="9">
+        <v>1</v>
+      </c>
+      <c r="J47" s="15">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+      <c r="O47">
+        <v>1</v>
+      </c>
+      <c r="P47" s="10"/>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A48" s="9"/>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48" s="10">
+        <v>1</v>
+      </c>
+      <c r="I48" s="9">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="L48">
+        <v>1</v>
+      </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <v>1</v>
+      </c>
+      <c r="P48" s="10"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="9"/>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49" s="10">
+        <v>1</v>
+      </c>
+      <c r="I49" s="9">
+        <v>1</v>
+      </c>
+      <c r="J49" s="15">
+        <v>1</v>
+      </c>
+      <c r="O49">
+        <v>1</v>
+      </c>
+      <c r="P49" s="10"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" s="9"/>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="H50" s="10">
+        <v>1</v>
+      </c>
+      <c r="I50" s="9"/>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="O50">
+        <v>1</v>
+      </c>
+      <c r="P50" s="10"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" s="11"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12">
+        <v>1</v>
+      </c>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="13">
+        <v>1</v>
+      </c>
+      <c r="I51" s="11">
+        <v>1</v>
+      </c>
+      <c r="J51" s="12"/>
+      <c r="K51" s="12"/>
+      <c r="L51" s="12"/>
+      <c r="M51" s="12"/>
+      <c r="N51" s="12">
+        <v>1</v>
+      </c>
+      <c r="O51" s="12"/>
+      <c r="P51" s="13"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:P16">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19:P34">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36:P51">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>